<commit_message>
forgot to turn off vpn redid renton data
</commit_message>
<xml_diff>
--- a/latency data.xlsx
+++ b/latency data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="40" windowWidth="28800" windowHeight="12220"/>
+    <workbookView xWindow="10940" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,11 +354,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2113841496"/>
-        <c:axId val="2111709800"/>
+        <c:axId val="2140356568"/>
+        <c:axId val="2142667544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2113841496"/>
+        <c:axId val="2140356568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -456,12 +456,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2111709800"/>
+        <c:crossAx val="2142667544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2111709800"/>
+        <c:axId val="2142667544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -554,7 +554,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2113841496"/>
+        <c:crossAx val="2140356568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1449,7 +1449,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1460,7 +1460,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1503,7 +1503,7 @@
         <v>1.49</v>
       </c>
       <c r="I2">
-        <v>10.86</v>
+        <v>11.51</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1520,7 +1520,7 @@
         <v>1.19</v>
       </c>
       <c r="I3">
-        <v>10.95</v>
+        <v>14.67</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1537,7 +1537,7 @@
         <v>1.27</v>
       </c>
       <c r="I4">
-        <v>13.48</v>
+        <v>13.38</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1554,7 +1554,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="I5">
-        <v>11.66</v>
+        <v>14.08</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1571,7 +1571,7 @@
         <v>1.22</v>
       </c>
       <c r="I6">
-        <v>10.93</v>
+        <v>13.78</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1588,7 +1588,7 @@
         <v>1.21</v>
       </c>
       <c r="I7">
-        <v>12.91</v>
+        <v>14.32</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1605,7 +1605,7 @@
         <v>1.28</v>
       </c>
       <c r="I8">
-        <v>37.15</v>
+        <v>13.46</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1622,7 +1622,7 @@
         <v>1.35</v>
       </c>
       <c r="I9">
-        <v>10.51</v>
+        <v>13.31</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1639,7 +1639,7 @@
         <v>1.63</v>
       </c>
       <c r="I10">
-        <v>11.11</v>
+        <v>13.83</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1656,7 +1656,7 @@
         <v>1.37</v>
       </c>
       <c r="I11">
-        <v>20.37</v>
+        <v>13.31</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1673,7 +1673,7 @@
         <v>0.9</v>
       </c>
       <c r="I12">
-        <v>10.75</v>
+        <v>13.83</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1690,7 +1690,7 @@
         <v>1.01</v>
       </c>
       <c r="I13">
-        <v>20.37</v>
+        <v>13.07</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1707,7 +1707,7 @@
         <v>1.06</v>
       </c>
       <c r="I14">
-        <v>10.75</v>
+        <v>13.95</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1724,7 +1724,7 @@
         <v>1.05</v>
       </c>
       <c r="I15">
-        <v>15.67</v>
+        <v>13.38</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1741,7 +1741,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I16">
-        <v>10.95</v>
+        <v>12.86</v>
       </c>
     </row>
     <row r="17" spans="5:12">
@@ -1758,7 +1758,7 @@
         <v>1.02</v>
       </c>
       <c r="I17">
-        <v>22.3</v>
+        <v>13.26</v>
       </c>
     </row>
     <row r="18" spans="5:12">
@@ -1775,7 +1775,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="I18">
-        <v>27.31</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="19" spans="5:12">
@@ -1792,7 +1792,7 @@
         <v>1.4</v>
       </c>
       <c r="I19">
-        <v>31.49</v>
+        <v>13.96</v>
       </c>
     </row>
     <row r="20" spans="5:12">
@@ -1809,7 +1809,7 @@
         <v>1.61</v>
       </c>
       <c r="I20">
-        <v>44.82</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="5:12">
@@ -1826,7 +1826,7 @@
         <v>1.31</v>
       </c>
       <c r="I21">
-        <v>11.44</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="22" spans="5:12">
@@ -1844,7 +1844,7 @@
       </c>
       <c r="I22">
         <f>AVERAGE(I2:I21)</f>
-        <v>17.788999999999998</v>
+        <v>13.553000000000001</v>
       </c>
     </row>
     <row r="26" spans="5:12">

</xml_diff>

<commit_message>
Updated data to include North Seattle, created graphs
</commit_message>
<xml_diff>
--- a/latency data.xlsx
+++ b/latency data.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\NetworksFinalProject\drawboard\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10940" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="10944" yWindow="0" windowWidth="25596" windowHeight="16056"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Distance(Miles)</t>
   </si>
@@ -47,24 +52,36 @@
   <si>
     <t>Renton, WA</t>
   </si>
+  <si>
+    <t>North Seattle, WA</t>
+  </si>
+  <si>
+    <t>Ontario, Canada</t>
+  </si>
+  <si>
+    <t>Renton, Washington</t>
+  </si>
+  <si>
+    <t>North Seattle, Washington</t>
+  </si>
+  <si>
+    <t>CS Labs</t>
+  </si>
+  <si>
+    <t>Localhost</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -87,9 +104,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -156,6 +172,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -208,64 +244,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -313,7 +349,7 @@
                   <c:v>34.76</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>150.83</c:v>
+                  <c:v>150.83000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>11.07</c:v>
@@ -325,7 +361,7 @@
                   <c:v>18.02</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.08</c:v>
+                  <c:v>17.079999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>12.52</c:v>
@@ -354,11 +390,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2140356568"/>
-        <c:axId val="2142667544"/>
+        <c:axId val="186775096"/>
+        <c:axId val="186775880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2140356568"/>
+        <c:axId val="186775096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -418,6 +454,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -456,12 +512,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142667544"/>
+        <c:crossAx val="186775880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2142667544"/>
+        <c:axId val="186775880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -516,6 +572,26 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -554,9 +630,485 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140356568"/>
+        <c:crossAx val="186775096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Latency vs Distance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$G$26:$G$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1995.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$26:$H$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>28.420999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.553000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6094999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.236</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="235828184"/>
+        <c:axId val="235829360"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="235828184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance (miles)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="235829360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="235829360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Latenccy(ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="235828184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -643,6 +1195,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1159,20 +1751,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>201930</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>300990</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1186,6 +2281,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>718459</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>163287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>54430</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>87086</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1449,7 +2574,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1457,19 +2582,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="11" max="11" width="21.1640625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="9" max="10" width="18.44140625" customWidth="1"/>
+    <col min="11" max="11" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1488,8 +2616,11 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E2">
         <v>1</v>
       </c>
@@ -1505,8 +2636,11 @@
       <c r="I2">
         <v>11.51</v>
       </c>
+      <c r="J2">
+        <v>12.95</v>
+      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E3">
         <v>2</v>
       </c>
@@ -1522,8 +2656,11 @@
       <c r="I3">
         <v>14.67</v>
       </c>
+      <c r="J3">
+        <v>13.91</v>
+      </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E4">
         <v>3</v>
       </c>
@@ -1539,8 +2676,11 @@
       <c r="I4">
         <v>13.38</v>
       </c>
+      <c r="J4">
+        <v>11.366</v>
+      </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E5">
         <v>4</v>
       </c>
@@ -1556,8 +2696,11 @@
       <c r="I5">
         <v>14.08</v>
       </c>
+      <c r="J5">
+        <v>12.11</v>
+      </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E6">
         <v>5</v>
       </c>
@@ -1573,8 +2716,11 @@
       <c r="I6">
         <v>13.78</v>
       </c>
+      <c r="J6">
+        <v>12.61</v>
+      </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E7">
         <v>6</v>
       </c>
@@ -1590,8 +2736,11 @@
       <c r="I7">
         <v>14.32</v>
       </c>
+      <c r="J7">
+        <v>13.77</v>
+      </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E8">
         <v>7</v>
       </c>
@@ -1607,8 +2756,11 @@
       <c r="I8">
         <v>13.46</v>
       </c>
+      <c r="J8">
+        <v>13.297000000000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E9">
         <v>8</v>
       </c>
@@ -1624,8 +2776,11 @@
       <c r="I9">
         <v>13.31</v>
       </c>
+      <c r="J9">
+        <v>12.54</v>
+      </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E10">
         <v>9</v>
       </c>
@@ -1641,8 +2796,11 @@
       <c r="I10">
         <v>13.83</v>
       </c>
+      <c r="J10">
+        <v>13.39</v>
+      </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E11">
         <v>10</v>
       </c>
@@ -1658,8 +2816,11 @@
       <c r="I11">
         <v>13.31</v>
       </c>
+      <c r="J11">
+        <v>13.56</v>
+      </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E12">
         <v>11</v>
       </c>
@@ -1675,8 +2836,11 @@
       <c r="I12">
         <v>13.83</v>
       </c>
+      <c r="J12">
+        <v>11.74</v>
+      </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E13">
         <v>12</v>
       </c>
@@ -1692,8 +2856,11 @@
       <c r="I13">
         <v>13.07</v>
       </c>
+      <c r="J13">
+        <v>11.16</v>
+      </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E14">
         <v>13</v>
       </c>
@@ -1709,8 +2876,11 @@
       <c r="I14">
         <v>13.95</v>
       </c>
+      <c r="J14">
+        <v>12.85</v>
+      </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E15">
         <v>14</v>
       </c>
@@ -1726,8 +2896,11 @@
       <c r="I15">
         <v>13.38</v>
       </c>
+      <c r="J15">
+        <v>13.42</v>
+      </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E16">
         <v>15</v>
       </c>
@@ -1743,8 +2916,11 @@
       <c r="I16">
         <v>12.86</v>
       </c>
+      <c r="J16">
+        <v>13.12</v>
+      </c>
     </row>
-    <row r="17" spans="5:12">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E17">
         <v>16</v>
       </c>
@@ -1760,8 +2936,11 @@
       <c r="I17">
         <v>13.26</v>
       </c>
+      <c r="J17">
+        <v>13.63</v>
+      </c>
     </row>
-    <row r="18" spans="5:12">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E18">
         <v>17</v>
       </c>
@@ -1777,8 +2956,11 @@
       <c r="I18">
         <v>13.3</v>
       </c>
+      <c r="J18">
+        <v>12.63</v>
+      </c>
     </row>
-    <row r="19" spans="5:12">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E19">
         <v>18</v>
       </c>
@@ -1794,8 +2976,11 @@
       <c r="I19">
         <v>13.96</v>
       </c>
+      <c r="J19">
+        <v>12.2</v>
+      </c>
     </row>
-    <row r="20" spans="5:12">
+    <row r="20" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E20">
         <v>19</v>
       </c>
@@ -1811,8 +2996,11 @@
       <c r="I20">
         <v>14</v>
       </c>
+      <c r="J20">
+        <v>13.45</v>
+      </c>
     </row>
-    <row r="21" spans="5:12">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E21">
         <v>20</v>
       </c>
@@ -1828,8 +3016,11 @@
       <c r="I21">
         <v>13.8</v>
       </c>
+      <c r="J21">
+        <v>12.71</v>
+      </c>
     </row>
-    <row r="22" spans="5:12">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.3">
       <c r="F22">
         <f>AVERAGE(F2:F21)</f>
         <v>28.421000000000003</v>
@@ -1846,21 +3037,72 @@
         <f>AVERAGE(I2:I21)</f>
         <v>13.553000000000001</v>
       </c>
+      <c r="J22">
+        <f>AVERAGE(J2:J21)</f>
+        <v>12.820649999999997</v>
+      </c>
     </row>
-    <row r="26" spans="5:12">
-      <c r="K26" t="s">
+    <row r="25" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
         <v>6</v>
       </c>
-      <c r="L26" t="s">
+      <c r="H25" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="5:12" ht="17">
-      <c r="K27" s="1">
+    <row r="26" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26">
         <v>1995.3</v>
       </c>
-      <c r="L27">
+      <c r="H26">
         <v>28.420999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27">
+        <v>15</v>
+      </c>
+      <c r="H27">
+        <v>13.553000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28">
+        <v>1.5</v>
+      </c>
+      <c r="H28">
+        <v>12.82</v>
+      </c>
+    </row>
+    <row r="29" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29">
+        <v>0.1</v>
+      </c>
+      <c r="H29">
+        <v>6.6094999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1.236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>